<commit_message>
Re-run DPLKINV001-001 until DPLKINV001-013 and Scripting DPLKINV001-014 until DPLKINV001-016
</commit_message>
<xml_diff>
--- a/DPLKINV001-002 - Setup Kegiatan Investasi - General Tambah, Ubah, View Detil & Hapus Data/Report/Report/Default.xlsx
+++ b/DPLKINV001-002 - Setup Kegiatan Investasi - General Tambah, Ubah, View Detil & Hapus Data/Report/Report/Default.xlsx
@@ -467,13 +467,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,11 +683,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -709,60 +709,60 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1187,23 +1187,23 @@
       <c r="C2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>115</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -1215,10 +1215,10 @@
       <c r="M2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="7" t="s">
         <v>123</v>
       </c>
       <c r="P2" s="3"/>
@@ -1239,7 +1239,7 @@
       <c r="Y2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="Z2" s="20"/>
+      <c r="Z2" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1258,32 +1258,32 @@
       <selection activeCell="A7" sqref="A7:U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="32.7109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.078125" style="14" customWidth="1"/>
-    <col min="21" max="21" width="12" style="14" customWidth="1"/>
-    <col min="22" max="16384" width="9.078125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="32.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="26" customWidth="1"/>
+    <col min="10" max="10" width="15" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.078125" style="26" customWidth="1"/>
+    <col min="21" max="21" width="12" style="26" customWidth="1"/>
+    <col min="22" max="16384" width="9.078125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1">
+    <row r="1" customFormat="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" ht="135">
+    <row r="2" ht="122.5">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="I2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="20" t="s">
         <v>84</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -1391,22 +1391,22 @@
       <c r="N2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="7"/>
+      <c r="T2" s="6"/>
       <c r="U2" s="24"/>
     </row>
     <row r="3" ht="45">
@@ -1437,7 +1437,7 @@
       <c r="I3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="20" t="s">
         <v>84</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1448,13 +1448,13 @@
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="25"/>
+      <c r="U3" s="15"/>
     </row>
     <row r="4" ht="45">
       <c r="A4" s="5" t="s">
@@ -1484,7 +1484,7 @@
       <c r="I4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="20" t="s">
         <v>84</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1497,13 +1497,13 @@
       <c r="N4" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="25"/>
+      <c r="U4" s="15"/>
     </row>
     <row r="5" ht="45">
       <c r="A5" s="5" t="s">
@@ -1533,7 +1533,7 @@
       <c r="I5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="20" t="s">
         <v>84</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -1544,17 +1544,17 @@
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="25"/>
+      <c r="U5" s="15"/>
     </row>
-    <row r="6">
+    <row r="6" ht="15">
       <c r="A6" s="2"/>
-      <c r="B6" s="22"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1573,11 +1573,11 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="26"/>
+      <c r="U6" s="14"/>
     </row>
-    <row r="7">
+    <row r="7" ht="15">
       <c r="A7" s="2"/>
-      <c r="B7" s="22"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1596,7 +1596,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="26"/>
+      <c r="U7" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1633,49 +1633,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="9.078125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.140625" style="19" customWidth="1"/>
-    <col min="13" max="14" width="61" style="19" customWidth="1"/>
-    <col min="15" max="15" width="47" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="103.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="69.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="61" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="63.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="51" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="49.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="59.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="53.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="56.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="57.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="62.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="51.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="57.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="53.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="35.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="58.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.078125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="9.078125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.140625" style="16" customWidth="1"/>
+    <col min="13" max="14" width="61" style="16" customWidth="1"/>
+    <col min="15" max="15" width="47" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="103.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="61" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="63.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="51" style="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="49.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="59.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="53.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="56.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="57.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="58.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="51.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="57.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="58.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.078125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
@@ -1825,7 +1825,7 @@
       <c r="B2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="18">
         <v>192168132154</v>
       </c>
       <c r="D2" s="10" t="str">
@@ -1833,7 +1833,7 @@
         <v>Verifikasi Database DPLK</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="23"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="12" t="s">
         <v>74</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="17"/>
+      <c r="V2" s="13"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -1877,7 +1877,7 @@
       <c r="AQ2" s="9"/>
       <c r="AR2" s="9"/>
       <c r="AS2" s="9"/>
-      <c r="AT2" s="13"/>
+      <c r="AT2" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>